<commit_message>
Fix num ("comma" instead of "dot" -> German)
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815D480B-3D4E-4CE5-906B-861178DA3524}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBF1B81-8F56-4A1D-8FC8-152B9F936DBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16860" activeTab="3" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16860" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="104">
   <si>
     <t>berm.height_mm</t>
   </si>
@@ -411,12 +411,6 @@
   </si>
   <si>
     <t>0,6 -&gt; 0.5 - 0.75 (SWMM recommendation)</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.4</t>
   </si>
   <si>
     <t>250 (200-300)</t>
@@ -1212,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F4C19-D880-47FC-8424-E4A612FEC51C}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B2" sqref="A2:B2"/>
@@ -1239,40 +1233,40 @@
         <v>14</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
       <c r="G2" s="37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1295,10 +1289,10 @@
         <v>300</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1321,10 +1315,10 @@
         <v>0.05</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1350,7 +1344,7 @@
         <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1373,10 +1367,10 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1399,10 +1393,10 @@
         <v>500</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1416,10 +1410,10 @@
         <v>0.437</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1439,10 +1433,10 @@
         <v>0.105</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1462,10 +1456,10 @@
         <v>4.7E-2</v>
       </c>
       <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" t="s">
         <v>74</v>
-      </c>
-      <c r="H10" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1488,7 +1482,7 @@
         <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
@@ -1511,10 +1505,10 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1531,10 +1525,10 @@
         <v>4.7E-2</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1557,10 +1551,10 @@
         <v>250</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1583,7 +1577,7 @@
         <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1606,10 +1600,10 @@
         <v>7.43</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1632,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1649,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1726,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D521626-6D22-40E6-8B80-D0FD83C4D8B0}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView topLeftCell="D7" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1747,34 +1741,34 @@
         <v>14</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>89</v>
-      </c>
       <c r="K1" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L1" s="52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -1885,7 +1879,7 @@
         <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1923,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1961,7 +1955,7 @@
         <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -1999,7 +1993,7 @@
         <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -2037,7 +2031,7 @@
         <v>0.35</v>
       </c>
       <c r="L8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -2075,7 +2069,7 @@
         <v>0.05</v>
       </c>
       <c r="L9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
@@ -2113,7 +2107,7 @@
         <v>19</v>
       </c>
       <c r="L10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -2151,7 +2145,7 @@
         <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2189,7 +2183,7 @@
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -2227,7 +2221,7 @@
         <v>40</v>
       </c>
       <c r="L13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -2265,7 +2259,7 @@
         <v>49</v>
       </c>
       <c r="L14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -2303,7 +2297,7 @@
         <v>28</v>
       </c>
       <c r="L15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2336,13 +2330,13 @@
         <v>14</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2585,11 +2579,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B86D96-106F-4982-9DEA-D74BD4578FBB}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2610,22 +2604,22 @@
         <v>14</v>
       </c>
       <c r="C1" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>71</v>
-      </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -2773,7 +2767,7 @@
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
       <c r="H7" s="40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -3133,7 +3127,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -3143,21 +3137,21 @@
       <c r="B25" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>55</v>
+      <c r="C25" s="34">
+        <v>0.4</v>
+      </c>
+      <c r="D25" s="34">
+        <v>0.4</v>
+      </c>
+      <c r="E25" s="34">
+        <v>0.4</v>
       </c>
       <c r="F25" s="46"/>
-      <c r="G25" s="34" t="s">
-        <v>55</v>
+      <c r="G25" s="34">
+        <v>0.4</v>
       </c>
       <c r="H25" s="53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -3181,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -3205,7 +3199,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -3229,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -3279,25 +3273,25 @@
         <v>14</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -3326,8 +3320,8 @@
       <c r="B5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
-        <v>54</v>
+      <c r="D5">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
scenarios: add column "id_type_parameter"
for saving order of SWMM parameters
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92403D7D-FA5F-4B1C-9B1B-3116E012B7B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D9DB4E-1769-4605-A7B2-A62ED195484C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16860" activeTab="2" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="106">
   <si>
     <t>berm.height_mm</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>default_scenario</t>
+  </si>
+  <si>
+    <t>id_type_parameter</t>
   </si>
 </sst>
 </file>
@@ -1207,80 +1210,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F4C19-D880-47FC-8424-E4A612FEC51C}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.36328125" customWidth="1"/>
-    <col min="6" max="6" width="50.1796875" customWidth="1"/>
-    <col min="7" max="7" width="78" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" customWidth="1"/>
+    <col min="7" max="7" width="50.140625" customWidth="1"/>
+    <col min="8" max="8" width="78" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="I1" s="52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>300</v>
+      <c r="B3" s="22">
+        <v>1</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>0</v>
       </c>
       <c r="D3">
         <v>300</v>
@@ -1288,25 +1296,28 @@
       <c r="E3">
         <v>300</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3">
         <v>300</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="39">
+        <v>300</v>
+      </c>
+      <c r="H3" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22">
+        <v>2</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="39">
-        <v>0.05</v>
       </c>
       <c r="D4" s="39">
         <v>0.05</v>
@@ -1317,22 +1328,25 @@
       <c r="F4" s="39">
         <v>0.05</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="H4" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22">
+        <v>3</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>12</v>
-      </c>
-      <c r="C5">
-        <v>0.3</v>
       </c>
       <c r="D5">
         <v>0.3</v>
@@ -1343,22 +1357,25 @@
       <c r="F5">
         <v>0.3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>0.3</v>
+      </c>
+      <c r="H5" t="s">
         <v>52</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22">
+        <v>4</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>16</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1369,22 +1386,25 @@
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
         <v>59</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22">
+        <v>1</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>2</v>
-      </c>
-      <c r="C7">
-        <v>500</v>
       </c>
       <c r="D7">
         <v>500</v>
@@ -1395,22 +1415,25 @@
       <c r="F7">
         <v>500</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>500</v>
+      </c>
+      <c r="H7" t="s">
         <v>64</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22">
+        <v>2</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>3</v>
-      </c>
-      <c r="C8">
-        <v>0.437</v>
       </c>
       <c r="D8">
         <v>0.437</v>
@@ -1421,22 +1444,25 @@
       <c r="F8">
         <v>0.437</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8">
+        <v>0.437</v>
+      </c>
+      <c r="H8" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22">
+        <v>3</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>4</v>
-      </c>
-      <c r="C9" s="39">
-        <v>0.105</v>
       </c>
       <c r="D9" s="39">
         <v>0.105</v>
@@ -1447,22 +1473,25 @@
       <c r="F9" s="39">
         <v>0.105</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="39">
+        <v>0.105</v>
+      </c>
+      <c r="H9" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22">
+        <v>4</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>5</v>
-      </c>
-      <c r="C10">
-        <v>4.7E-2</v>
       </c>
       <c r="D10">
         <v>4.7E-2</v>
@@ -1473,22 +1502,25 @@
       <c r="F10">
         <v>4.7E-2</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H10" t="s">
         <v>72</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22">
+        <v>5</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>6</v>
-      </c>
-      <c r="C11">
-        <v>30</v>
       </c>
       <c r="D11">
         <v>30</v>
@@ -1499,19 +1531,22 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22">
+        <v>6</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>7</v>
-      </c>
-      <c r="C12">
-        <v>0.5</v>
       </c>
       <c r="D12">
         <v>0.5</v>
@@ -1522,22 +1557,25 @@
       <c r="F12">
         <v>0.5</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22">
+        <v>7</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>8</v>
-      </c>
-      <c r="C13">
-        <v>4.7E-2</v>
       </c>
       <c r="D13">
         <v>4.7E-2</v>
@@ -1548,101 +1586,113 @@
       <c r="F13">
         <v>4.7E-2</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H13" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22">
+        <v>1</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>250</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
       <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>250</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>54</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22">
+        <v>2</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
       <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>0.6</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
       <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>0.6</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>53</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22">
+        <v>3</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
       <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>7.43</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
       <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>7.43</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>55</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22">
+        <v>4</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
       <c r="D17">
         <v>0</v>
       </c>
@@ -1652,88 +1702,109 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22">
+        <v>1</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>2</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>2</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22">
+        <v>2</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.5</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22">
+        <v>3</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>100</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="22">
+        <v>4</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22">
+        <v>5</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="22">
+        <v>6</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1745,67 +1816,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D521626-6D22-40E6-8B80-D0FD83C4D8B0}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="48.81640625" customWidth="1"/>
-    <col min="6" max="10" width="45.453125" customWidth="1"/>
-    <col min="11" max="12" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="48.85546875" customWidth="1"/>
+    <col min="7" max="11" width="45.42578125" customWidth="1"/>
+    <col min="12" max="13" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="M1" s="52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="15">
@@ -1815,13 +1890,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="15">
+        <v>0</v>
+      </c>
+      <c r="G2" s="15">
         <v>100</v>
       </c>
-      <c r="G2" s="15">
-        <v>0</v>
-      </c>
       <c r="H2" s="15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I2" s="15">
         <v>100</v>
@@ -1829,19 +1904,22 @@
       <c r="J2" s="15">
         <v>100</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="15">
+        <v>100</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0.15</v>
       </c>
       <c r="D3" s="8">
         <v>0.15</v>
@@ -1867,19 +1945,22 @@
       <c r="K3" s="8">
         <v>0.15</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0.1</v>
       </c>
       <c r="D4" s="9">
         <v>0.1</v>
@@ -1902,23 +1983,26 @@
       <c r="J4" s="9">
         <v>0.1</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
       <c r="D5" s="8">
         <v>0</v>
       </c>
@@ -1943,57 +2027,63 @@
       <c r="K5" s="8">
         <v>0</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C6" s="11">
-        <v>80</v>
       </c>
       <c r="D6" s="11">
         <v>80</v>
       </c>
       <c r="E6" s="11">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="F6" s="11">
         <v>160</v>
       </c>
       <c r="G6" s="11">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="H6" s="11">
         <v>80</v>
       </c>
       <c r="I6" s="11">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="J6" s="11">
         <v>160</v>
       </c>
       <c r="K6" s="11">
+        <v>160</v>
+      </c>
+      <c r="L6" s="11">
         <v>80</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C7" s="15">
-        <v>0.65</v>
       </c>
       <c r="D7" s="15">
         <v>0.65</v>
@@ -2016,22 +2106,25 @@
       <c r="J7" s="15">
         <v>0.65</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="15">
+        <v>0.65</v>
+      </c>
+      <c r="L7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C8" s="8">
-        <v>0.35</v>
       </c>
       <c r="D8" s="8">
         <v>0.35</v>
@@ -2057,19 +2150,22 @@
       <c r="K8" s="8">
         <v>0.35</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="M8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.05</v>
       </c>
       <c r="D9" s="8">
         <v>0.05</v>
@@ -2095,19 +2191,22 @@
       <c r="K9" s="8">
         <v>0.05</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="M9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C10" s="8">
-        <v>90</v>
       </c>
       <c r="D10" s="8">
         <v>90</v>
@@ -2130,22 +2229,25 @@
       <c r="J10" s="8">
         <v>90</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="8">
+        <v>90</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C11" s="8">
-        <v>30</v>
       </c>
       <c r="D11" s="8">
         <v>30</v>
@@ -2171,19 +2273,22 @@
       <c r="K11" s="8">
         <v>30</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="8">
+        <v>30</v>
+      </c>
+      <c r="M11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="16">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C12" s="17">
-        <v>10</v>
       </c>
       <c r="D12" s="17">
         <v>10</v>
@@ -2209,57 +2314,63 @@
       <c r="K12" s="17">
         <v>10</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="17">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="13">
-        <v>0</v>
-      </c>
       <c r="D13" s="13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13">
         <v>40</v>
       </c>
-      <c r="E13" s="13">
+      <c r="F13" s="13">
         <v>80</v>
       </c>
-      <c r="F13" s="13">
-        <v>0</v>
-      </c>
       <c r="G13" s="13">
         <v>0</v>
       </c>
       <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
         <v>40</v>
       </c>
-      <c r="I13" s="13">
+      <c r="J13" s="13">
         <v>80</v>
       </c>
-      <c r="J13" s="13">
-        <v>0</v>
-      </c>
       <c r="K13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13">
         <v>40</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0.6</v>
       </c>
       <c r="D14" s="8">
         <v>0.6</v>
@@ -2282,22 +2393,25 @@
       <c r="J14" s="8">
         <v>0.6</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.1</v>
       </c>
       <c r="D15" s="8">
         <v>0.1</v>
@@ -2320,10 +2434,13 @@
       <c r="J15" s="8">
         <v>0.1</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2335,267 +2452,334 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D31D51-F65D-4CB7-BD89-E3C799A8A144}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" customWidth="1"/>
-    <col min="3" max="3" width="25.26953125" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="F1" s="54" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="22">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="23"/>
       <c r="E2" s="19"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="19"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22">
+        <v>3</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="19"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="19"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22">
+        <v>4</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="19"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="19"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22">
+        <v>1</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="19"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22">
+        <v>2</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="19"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="19"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22">
+        <v>3</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="19"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="19"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22">
+        <v>4</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="19"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="19"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22">
+        <v>5</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="19"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22">
+        <v>6</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="19"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="19"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22">
+        <v>7</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="19"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22">
+        <v>1</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="19"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22">
+        <v>2</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="19"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="19"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22">
+        <v>4</v>
+      </c>
+      <c r="C16" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="19"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22">
+        <v>1</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="19"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22">
+        <v>2</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="19"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="19"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22">
+        <v>3</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="19"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="19"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22">
+        <v>4</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="19"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="19"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="22">
+        <v>5</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="19"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="22">
+        <v>6</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="19"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2604,59 +2788,64 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B86D96-106F-4982-9DEA-D74BD4578FBB}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.90625" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.81640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.36328125" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.90625" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="D1" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="H1" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="23">
+      <c r="B2" s="22">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="23">
@@ -2671,18 +2860,21 @@
       <c r="G2" s="23">
         <v>0</v>
       </c>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2" s="23">
+        <v>0</v>
+      </c>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23">
-        <v>0</v>
-      </c>
       <c r="D3" s="23">
         <v>0</v>
       </c>
@@ -2695,17 +2887,20 @@
       <c r="G3" s="23">
         <v>0</v>
       </c>
-      <c r="H3" s="27"/>
-    </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="H3" s="23">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22">
+        <v>3</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="23">
-        <v>0.12</v>
       </c>
       <c r="D4" s="23">
         <v>0.12</v>
@@ -2719,19 +2914,22 @@
       <c r="G4" s="23">
         <v>0.12</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="I4" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22">
+        <v>4</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="23">
-        <v>2.5</v>
       </c>
       <c r="D5" s="23">
         <v>2.5</v>
@@ -2745,19 +2943,22 @@
       <c r="G5" s="23">
         <v>2.5</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="23">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="27">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22">
+        <v>1</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>2</v>
-      </c>
-      <c r="C6" s="32">
-        <v>80</v>
       </c>
       <c r="D6" s="32">
         <v>80</v>
@@ -2771,19 +2972,22 @@
       <c r="G6" s="32">
         <v>80</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="32">
+        <v>80</v>
+      </c>
+      <c r="I6" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22">
+        <v>2</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" s="23">
-        <v>0.16500000000000001</v>
       </c>
       <c r="D7" s="23">
         <v>0.16500000000000001</v>
@@ -2791,64 +2995,83 @@
       <c r="E7" s="23">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="23">
+        <v>0.16500000000000001</v>
+      </c>
       <c r="G7" s="23"/>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="23"/>
+      <c r="I7" s="40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22">
+        <v>3</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="28" t="s">
+      <c r="D8" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="F8" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="G8" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="I8" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22">
+        <v>4</v>
+      </c>
+      <c r="C9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="32">
+      <c r="D9" s="32">
         <v>45</v>
       </c>
-      <c r="D9" s="32">
+      <c r="E9" s="32">
         <v>90</v>
-      </c>
-      <c r="E9" s="43">
-        <v>180</v>
       </c>
       <c r="F9" s="43">
         <v>180</v>
       </c>
       <c r="G9" s="43">
+        <v>180</v>
+      </c>
+      <c r="H9" s="43">
         <v>360</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="I9" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22">
+        <v>5</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="32">
-        <v>0</v>
-      </c>
       <c r="D10" s="32">
         <v>0</v>
       </c>
@@ -2858,23 +3081,26 @@
       <c r="F10" s="32">
         <v>0</v>
       </c>
-      <c r="G10" s="44">
-        <v>0</v>
-      </c>
-      <c r="H10" s="25" t="s">
+      <c r="G10" s="32">
+        <v>0</v>
+      </c>
+      <c r="H10" s="44">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22">
+        <v>6</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="32">
-        <v>0</v>
-      </c>
       <c r="D11" s="32">
         <v>0</v>
       </c>
@@ -2887,20 +3113,23 @@
       <c r="G11" s="32">
         <v>0</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="32">
+        <v>0</v>
+      </c>
+      <c r="I11" s="30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22">
+        <v>7</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="32">
-        <v>0</v>
-      </c>
       <c r="D12" s="32">
         <v>0</v>
       </c>
@@ -2913,131 +3142,155 @@
       <c r="G12" s="32">
         <v>0</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="32">
+        <v>0</v>
+      </c>
+      <c r="I12" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22">
+        <v>1</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="33"/>
       <c r="D13" s="33"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="53" t="s">
+      <c r="E13" s="33"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22">
+        <v>2</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="34"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="53" t="s">
+      <c r="E14" s="34"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22">
+        <v>3</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="34"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="53" t="s">
+      <c r="E15" s="34"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22">
+        <v>4</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="34"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="53" t="s">
+      <c r="E16" s="34"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22">
+        <v>5</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="34"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="53" t="s">
+      <c r="E17" s="34"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22">
+        <v>6</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="34"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="53" t="s">
+      <c r="E18" s="34"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22">
+        <v>7</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="35"/>
       <c r="D19" s="35"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="53" t="s">
+      <c r="E19" s="35"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="53" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22">
+        <v>1</v>
+      </c>
+      <c r="C20" s="23" t="s">
         <v>2</v>
-      </c>
-      <c r="C20" s="32">
-        <v>350</v>
       </c>
       <c r="D20" s="32">
         <v>350</v>
@@ -3051,19 +3304,22 @@
       <c r="G20" s="32">
         <v>350</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="32">
+        <v>350</v>
+      </c>
+      <c r="I20" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22">
+        <v>2</v>
+      </c>
+      <c r="C21" s="23" t="s">
         <v>21</v>
-      </c>
-      <c r="C21" s="32">
-        <v>0.3</v>
       </c>
       <c r="D21" s="32">
         <v>0.3</v>
@@ -3077,19 +3333,22 @@
       <c r="G21" s="32">
         <v>0.3</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="I21" s="29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="23" t="s">
         <v>30</v>
-      </c>
-      <c r="C22" s="32">
-        <v>1.8</v>
       </c>
       <c r="D22" s="32">
         <v>1.8</v>
@@ -3103,20 +3362,23 @@
       <c r="G22" s="32">
         <v>1.8</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="32">
+        <v>1.8</v>
+      </c>
+      <c r="I22" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="22">
+        <v>4</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="33">
-        <v>0</v>
-      </c>
       <c r="D23" s="33">
         <v>0</v>
       </c>
@@ -3129,19 +3391,22 @@
       <c r="G23" s="33">
         <v>0</v>
       </c>
-      <c r="H23" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+      <c r="I23" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="22">
+        <v>1</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>31</v>
-      </c>
-      <c r="C24" s="33">
-        <v>1</v>
       </c>
       <c r="D24" s="33">
         <v>1</v>
@@ -3149,23 +3414,26 @@
       <c r="E24" s="33">
         <v>1</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="33">
+      <c r="F24" s="33">
         <v>1</v>
       </c>
-      <c r="H24" s="53" t="s">
+      <c r="G24" s="45"/>
+      <c r="H24" s="33">
+        <v>1</v>
+      </c>
+      <c r="I24" s="53" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="22">
+        <v>2</v>
+      </c>
+      <c r="C25" s="24" t="s">
         <v>32</v>
-      </c>
-      <c r="C25" s="34">
-        <v>0.4</v>
       </c>
       <c r="D25" s="34">
         <v>0.4</v>
@@ -3173,102 +3441,117 @@
       <c r="E25" s="34">
         <v>0.4</v>
       </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="34">
+      <c r="F25" s="34">
         <v>0.4</v>
       </c>
-      <c r="H25" s="53" t="s">
+      <c r="G25" s="46"/>
+      <c r="H25" s="34">
+        <v>0.4</v>
+      </c>
+      <c r="I25" s="53" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22">
+        <v>3</v>
+      </c>
+      <c r="C26" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="34">
-        <v>0</v>
-      </c>
       <c r="D26" s="34">
         <v>0</v>
       </c>
       <c r="E26" s="34">
         <v>0</v>
       </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="34">
-        <v>0</v>
-      </c>
-      <c r="H26" s="53" t="s">
+      <c r="F26" s="34">
+        <v>0</v>
+      </c>
+      <c r="G26" s="46"/>
+      <c r="H26" s="34">
+        <v>0</v>
+      </c>
+      <c r="I26" s="53" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="22">
+        <v>4</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="34">
-        <v>0</v>
-      </c>
       <c r="D27" s="34">
         <v>0</v>
       </c>
       <c r="E27" s="34">
         <v>0</v>
       </c>
-      <c r="F27" s="46"/>
-      <c r="G27" s="34">
-        <v>0</v>
-      </c>
-      <c r="H27" s="53" t="s">
+      <c r="F27" s="34">
+        <v>0</v>
+      </c>
+      <c r="G27" s="46"/>
+      <c r="H27" s="34">
+        <v>0</v>
+      </c>
+      <c r="I27" s="53" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="22">
+        <v>5</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="34">
-        <v>0</v>
-      </c>
       <c r="D28" s="34">
         <v>0</v>
       </c>
       <c r="E28" s="34">
         <v>0</v>
       </c>
-      <c r="F28" s="46"/>
-      <c r="G28" s="34">
-        <v>0</v>
-      </c>
-      <c r="H28" s="53" t="s">
+      <c r="F28" s="34">
+        <v>0</v>
+      </c>
+      <c r="G28" s="46"/>
+      <c r="H28" s="34">
+        <v>0</v>
+      </c>
+      <c r="I28" s="53" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22">
+        <v>6</v>
+      </c>
+      <c r="C29" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="35"/>
       <c r="D29" s="35"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="51"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="47"/>
       <c r="H29" s="51"/>
-    </row>
-    <row r="47" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L47" s="6"/>
+      <c r="I29" s="51"/>
+    </row>
+    <row r="47" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M47" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3278,114 +3561,140 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D226361B-E2F4-480B-BE87-D86C9E2C81ED}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="F1" s="52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22">
+        <v>1</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="22">
+        <v>3</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22">
+        <v>4</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22">
+        <v>5</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22">
+        <v>6</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Apply for all permeable pavements scenarios
and fix parameterisation file
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D9DB4E-1769-4605-A7B2-A62ED195484C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21546D67-C924-482E-B190-9717D0038FBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" activeTab="3" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -1212,27 +1212,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F4C19-D880-47FC-8424-E4A612FEC51C}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.42578125" customWidth="1"/>
-    <col min="7" max="7" width="50.140625" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.453125" customWidth="1"/>
+    <col min="7" max="7" width="50.1796875" customWidth="1"/>
     <col min="8" max="8" width="78" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>102</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>10</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>10</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>27</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>29</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>29</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>29</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>29</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>29</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>29</v>
       </c>
@@ -1822,17 +1822,17 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="48.85546875" customWidth="1"/>
-    <col min="7" max="11" width="45.42578125" customWidth="1"/>
-    <col min="12" max="13" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="48.81640625" customWidth="1"/>
+    <col min="7" max="11" width="45.453125" customWidth="1"/>
+    <col min="12" max="13" width="48.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
@@ -2458,16 +2458,16 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
@@ -2501,7 +2501,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
@@ -2515,7 +2515,7 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
@@ -2529,7 +2529,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>10</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>10</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
@@ -2585,7 +2585,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>10</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
@@ -2627,7 +2627,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>10</v>
       </c>
@@ -2641,7 +2641,7 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>27</v>
       </c>
@@ -2655,7 +2655,7 @@
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
@@ -2669,7 +2669,7 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>27</v>
       </c>
@@ -2683,7 +2683,7 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>27</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>29</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>29</v>
       </c>
@@ -2725,7 +2725,7 @@
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>29</v>
       </c>
@@ -2739,7 +2739,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>29</v>
       </c>
@@ -2753,7 +2753,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>29</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>29</v>
       </c>
@@ -2790,26 +2790,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B86D96-106F-4982-9DEA-D74BD4578FBB}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.81640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" style="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.81640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>9</v>
       </c>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="I2" s="27"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
@@ -2892,7 +2892,7 @@
       </c>
       <c r="I3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>20</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>20</v>
       </c>
@@ -2998,13 +2998,17 @@
       <c r="F7" s="23">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="23">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0.16500000000000001</v>
+      </c>
       <c r="I7" s="40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>20</v>
       </c>
@@ -3033,7 +3037,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
@@ -3062,7 +3066,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
@@ -3091,7 +3095,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>20</v>
       </c>
@@ -3120,7 +3124,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>20</v>
       </c>
@@ -3149,7 +3153,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
@@ -3168,7 +3172,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>10</v>
       </c>
@@ -3187,7 +3191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>10</v>
       </c>
@@ -3206,7 +3210,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>10</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>10</v>
       </c>
@@ -3244,7 +3248,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>10</v>
       </c>
@@ -3263,7 +3267,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>10</v>
       </c>
@@ -3282,7 +3286,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>27</v>
       </c>
@@ -3311,7 +3315,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>27</v>
       </c>
@@ -3340,7 +3344,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>27</v>
       </c>
@@ -3369,7 +3373,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>27</v>
       </c>
@@ -3398,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>29</v>
       </c>
@@ -3425,7 +3429,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
         <v>29</v>
       </c>
@@ -3452,7 +3456,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
         <v>29</v>
       </c>
@@ -3479,7 +3483,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>29</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
         <v>29</v>
       </c>
@@ -3533,7 +3537,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
         <v>29</v>
       </c>
@@ -3550,7 +3554,7 @@
       <c r="H29" s="51"/>
       <c r="I29" s="51"/>
     </row>
-    <row r="47" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M47" s="6"/>
     </row>
   </sheetData>
@@ -3567,16 +3571,16 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
@@ -3596,7 +3600,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>102</v>
       </c>
@@ -3609,7 +3613,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>27</v>
       </c>
@@ -3623,7 +3627,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>29</v>
       </c>
@@ -3634,7 +3638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>29</v>
       </c>
@@ -3648,7 +3652,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>29</v>
       </c>
@@ -3659,7 +3663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>29</v>
       </c>
@@ -3673,7 +3677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>29</v>
       </c>
@@ -3687,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Fix :bug: for LID green_roof
* drainage mat needs to be thicker than 0 (set to 0.1mm of simulated without)
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27D9412-B4AD-4A0A-8197-751013ADF1EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E19C8A6-A007-4282-A2BC-03891DB893EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" activeTab="3" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" activeTab="1" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -663,7 +663,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -753,15 +753,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -774,9 +795,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -897,6 +915,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1215,7 +1239,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E14" sqref="E14:E17"/>
@@ -1235,47 +1259,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="48" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>62</v>
       </c>
       <c r="I2" t="s">
@@ -1283,13 +1307,13 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="19">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D3">
@@ -1301,10 +1325,10 @@
       <c r="F3">
         <v>300</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="35">
         <v>300</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="I3" t="s">
@@ -1312,28 +1336,28 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="35">
         <v>0.05</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="35">
         <v>0.05</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="35">
         <v>0.05</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="35">
         <v>0.05</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="35" t="s">
         <v>58</v>
       </c>
       <c r="I4" t="s">
@@ -1341,13 +1365,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D5">
@@ -1370,13 +1394,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>4</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D6">
@@ -1399,13 +1423,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D7">
@@ -1428,13 +1452,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <v>2</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D8">
@@ -1449,7 +1473,7 @@
       <c r="G8">
         <v>0.437</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="35" t="s">
         <v>60</v>
       </c>
       <c r="I8" t="s">
@@ -1457,28 +1481,28 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="19">
         <v>3</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="35">
         <v>0.105</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="35">
         <v>0.105</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="35">
         <v>0.105</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="35">
         <v>0.105</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="35" t="s">
         <v>64</v>
       </c>
       <c r="I9" t="s">
@@ -1486,13 +1510,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="19">
         <v>4</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D10">
@@ -1515,13 +1539,13 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="19">
         <v>5</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D11">
@@ -1541,13 +1565,13 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="19">
         <v>6</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D12">
@@ -1562,7 +1586,7 @@
       <c r="G12">
         <v>0.5</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="35" t="s">
         <v>74</v>
       </c>
       <c r="I12" t="s">
@@ -1570,13 +1594,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="19">
         <v>7</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D13">
@@ -1591,7 +1615,7 @@
       <c r="G13">
         <v>4.7E-2</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="35" t="s">
         <v>75</v>
       </c>
       <c r="I13" t="s">
@@ -1599,13 +1623,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="19">
         <v>1</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>2</v>
       </c>
       <c r="F14">
@@ -1622,13 +1646,13 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="19">
         <v>2</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F15">
@@ -1645,13 +1669,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="19">
         <v>3</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>30</v>
       </c>
       <c r="F16">
@@ -1668,13 +1692,13 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="19">
         <v>4</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="21" t="s">
         <v>24</v>
       </c>
       <c r="F17">
@@ -1688,13 +1712,13 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="19">
         <v>1</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="21" t="s">
         <v>31</v>
       </c>
       <c r="E18">
@@ -1708,13 +1732,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="19">
         <v>2</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="21" t="s">
         <v>32</v>
       </c>
       <c r="E19">
@@ -1725,13 +1749,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="19">
         <v>3</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="21" t="s">
         <v>33</v>
       </c>
       <c r="E20">
@@ -1742,13 +1766,13 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="19">
         <v>4</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E21">
@@ -1759,13 +1783,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="19">
         <v>5</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="21" t="s">
         <v>35</v>
       </c>
       <c r="E22">
@@ -1776,13 +1800,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="19">
         <v>6</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="21" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1796,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D521626-6D22-40E6-8B80-D0FD83C4D8B0}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1811,119 +1835,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="48" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="15">
-        <v>0</v>
-      </c>
-      <c r="E2" s="15">
-        <v>0</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0</v>
-      </c>
-      <c r="G2" s="15">
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
         <v>100</v>
       </c>
-      <c r="H2" s="15">
-        <v>0</v>
-      </c>
-      <c r="I2" s="15">
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13">
         <v>100</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="13">
         <v>100</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="13">
         <v>100</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.15</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>0.15</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>0.15</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>0.15</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>0.15</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>0.15</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <v>0.15</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <v>0.15</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>0.15</v>
       </c>
       <c r="M3" t="s">
@@ -1931,204 +1955,204 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>0.1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.1</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>0.1</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.1</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>0.1</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>0.1</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>0.1</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <v>0.1</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="8" t="s">
         <v>50</v>
       </c>
       <c r="M4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8">
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
         <v>0</v>
       </c>
       <c r="M5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="52">
+        <v>1</v>
+      </c>
+      <c r="C6" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="54">
         <v>80</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="54">
         <v>80</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="54">
         <v>160</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="54">
         <v>160</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="54">
         <v>80</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="54">
         <v>80</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="54">
         <v>160</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="54">
         <v>160</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="54">
         <v>80</v>
       </c>
       <c r="M6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="7">
         <v>0.65</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="7">
         <v>0.65</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="7">
         <v>0.65</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="7">
         <v>0.65</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="7">
         <v>0.65</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="7">
         <v>0.65</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="7">
         <v>0.65</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="7">
         <v>0.65</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="55" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7">
-        <v>2</v>
+      <c r="B8" s="6">
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0.35</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>0.35</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>0.35</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>0.35</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>0.35</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>0.35</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <v>0.35</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>0.35</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>0.35</v>
       </c>
       <c r="M8" t="s">
@@ -2136,40 +2160,40 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7">
-        <v>3</v>
+      <c r="B9" s="6">
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>0.05</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>0.05</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>0.05</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>0.05</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>0.05</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>0.05</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <v>0.05</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>0.05</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>0.05</v>
       </c>
       <c r="M9" t="s">
@@ -2177,40 +2201,40 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7">
-        <v>4</v>
+      <c r="B10" s="6">
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>90</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>90</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>90</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>90</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>90</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>90</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <v>90</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <v>90</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="M10" t="s">
@@ -2218,40 +2242,40 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
-        <v>5</v>
+      <c r="B11" s="6">
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>30</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>30</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>30</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>30</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <v>30</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>30</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <v>30</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="7">
         <v>30</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="7">
         <v>30</v>
       </c>
       <c r="M11" t="s">
@@ -2259,40 +2283,40 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="16">
-        <v>6</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="14">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="15">
         <v>10</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="15">
         <v>10</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="15">
         <v>10</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="15">
         <v>10</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="15">
         <v>10</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="15">
         <v>10</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="15">
         <v>10</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="15">
         <v>10</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="15">
         <v>10</v>
       </c>
       <c r="M12" t="s">
@@ -2300,40 +2324,40 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13">
+      <c r="D13" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="11">
         <v>40</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="11">
         <v>80</v>
       </c>
-      <c r="G13" s="13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="13">
+      <c r="G13" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="11">
         <v>40</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="11">
         <v>80</v>
       </c>
-      <c r="K13" s="13">
-        <v>0</v>
-      </c>
-      <c r="L13" s="13">
+      <c r="K13" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="11">
         <v>40</v>
       </c>
       <c r="M13" t="s">
@@ -2341,40 +2365,40 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>0.6</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>0.6</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>0.6</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>0.6</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <v>0.6</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>0.6</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="7">
         <v>0.6</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <v>0.6</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="7" t="s">
         <v>49</v>
       </c>
       <c r="M14" t="s">
@@ -2382,40 +2406,40 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>0.1</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>0.1</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>0.1</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>0.1</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <v>0.1</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>0.1</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <v>0.1</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="7">
         <v>0.1</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="M15" t="s">
@@ -2443,37 +2467,37 @@
   <cols>
     <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.81640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.81640625" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.81640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.81640625" style="44" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="62.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="37" t="s">
         <v>68</v>
       </c>
       <c r="I1" t="s">
@@ -2481,723 +2505,723 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="19">
         <v>1</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="22">
-        <v>0</v>
-      </c>
-      <c r="E2" s="22">
-        <v>0</v>
-      </c>
-      <c r="F2" s="22">
-        <v>0</v>
-      </c>
-      <c r="G2" s="22">
-        <v>0</v>
-      </c>
-      <c r="H2" s="22">
-        <v>0</v>
-      </c>
-      <c r="I2" s="25"/>
+      <c r="C2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <v>0</v>
+      </c>
+      <c r="E2" s="20">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20">
+        <v>0</v>
+      </c>
+      <c r="G2" s="20">
+        <v>0</v>
+      </c>
+      <c r="H2" s="20">
+        <v>0</v>
+      </c>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="19">
         <v>2</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22">
-        <v>0</v>
-      </c>
-      <c r="E3" s="22">
-        <v>0</v>
-      </c>
-      <c r="F3" s="22">
-        <v>0</v>
-      </c>
-      <c r="G3" s="22">
-        <v>0</v>
-      </c>
-      <c r="H3" s="22">
-        <v>0</v>
-      </c>
-      <c r="I3" s="25"/>
+      <c r="D3" s="20">
+        <v>0</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20">
+        <v>0</v>
+      </c>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>3</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <v>0.12</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>0.12</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <v>0.12</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <v>0.12</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="20">
         <v>0.12</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>4</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="20">
         <v>2.5</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="20">
         <v>2.5</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <v>2.5</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="20">
         <v>2.5</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="20">
         <v>2.5</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="28">
         <v>80</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>80</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="28">
         <v>80</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="28">
         <v>80</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="28">
         <v>80</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="20">
         <v>0.16500000000000001</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="20">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="20">
         <v>0.16500000000000001</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="20">
         <v>0.16500000000000001</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="36" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="38">
         <v>0.85</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="38">
         <v>0.85</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="38">
         <v>0.85</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="38">
         <v>0.85</v>
       </c>
-      <c r="H8" s="40">
+      <c r="H8" s="38">
         <v>0.85</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="24" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="19">
         <v>4</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="28">
         <v>45</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="28">
         <v>90</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="39">
         <v>180</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="39">
         <v>180</v>
       </c>
-      <c r="H9" s="41">
+      <c r="H9" s="39">
         <v>360</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="19">
         <v>5</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="30">
-        <v>0</v>
-      </c>
-      <c r="E10" s="30">
-        <v>0</v>
-      </c>
-      <c r="F10" s="30">
-        <v>0</v>
-      </c>
-      <c r="G10" s="30">
-        <v>0</v>
-      </c>
-      <c r="H10" s="42">
-        <v>0</v>
-      </c>
-      <c r="I10" s="24" t="s">
+      <c r="D10" s="28">
+        <v>0</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="28">
+        <v>0</v>
+      </c>
+      <c r="H10" s="40">
+        <v>0</v>
+      </c>
+      <c r="I10" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="19">
         <v>6</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="30">
-        <v>0</v>
-      </c>
-      <c r="E11" s="30">
-        <v>0</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0</v>
-      </c>
-      <c r="G11" s="30">
-        <v>0</v>
-      </c>
-      <c r="H11" s="30">
-        <v>0</v>
-      </c>
-      <c r="I11" s="28" t="s">
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0</v>
+      </c>
+      <c r="H11" s="28">
+        <v>0</v>
+      </c>
+      <c r="I11" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="19">
         <v>7</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="30">
-        <v>0</v>
-      </c>
-      <c r="E12" s="30">
-        <v>0</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0</v>
-      </c>
-      <c r="G12" s="30">
-        <v>0</v>
-      </c>
-      <c r="H12" s="30">
-        <v>0</v>
-      </c>
-      <c r="I12" s="28" t="s">
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+      <c r="I12" s="26" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="19">
         <v>1</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="51" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="19">
         <v>2</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="51" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="19">
         <v>3</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="51" t="s">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="19">
         <v>4</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="51" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="19">
         <v>5</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="51" t="s">
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="19">
         <v>6</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="51" t="s">
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="19">
         <v>7</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="51" t="s">
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="49" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="19">
         <v>1</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="28">
         <v>350</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>350</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="28">
         <v>350</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="28">
         <v>350</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="28">
         <v>350</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="19">
         <v>2</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="28">
         <v>0.3</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="28">
         <v>0.3</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="28">
         <v>0.3</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="28">
         <v>0.3</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="28">
         <v>0.3</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="25" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="19">
         <v>3</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="28">
         <v>1.8</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="28">
         <v>1.8</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="28">
         <v>1.8</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="28">
         <v>1.8</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="28">
         <v>1.8</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="18" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="19">
         <v>4</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="31">
-        <v>0</v>
-      </c>
-      <c r="E23" s="31">
-        <v>0</v>
-      </c>
-      <c r="F23" s="31">
-        <v>0</v>
-      </c>
-      <c r="G23" s="31">
-        <v>0</v>
-      </c>
-      <c r="H23" s="31">
-        <v>0</v>
-      </c>
-      <c r="I23" s="29">
+      <c r="D23" s="29">
+        <v>0</v>
+      </c>
+      <c r="E23" s="29">
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
+        <v>0</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+      <c r="H23" s="29">
+        <v>0</v>
+      </c>
+      <c r="I23" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="19">
         <v>1</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="29">
         <v>1</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="29">
         <v>1</v>
       </c>
-      <c r="F24" s="31">
+      <c r="F24" s="29">
         <v>1</v>
       </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="31">
+      <c r="G24" s="41"/>
+      <c r="H24" s="29">
         <v>1</v>
       </c>
-      <c r="I24" s="51" t="s">
+      <c r="I24" s="49" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="19">
         <v>2</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="30">
         <v>0.4</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="30">
         <v>0.4</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="30">
         <v>0.4</v>
       </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="32">
+      <c r="G25" s="42"/>
+      <c r="H25" s="30">
         <v>0.4</v>
       </c>
-      <c r="I25" s="51" t="s">
+      <c r="I25" s="49" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="19">
         <v>3</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="32">
-        <v>0</v>
-      </c>
-      <c r="E26" s="32">
-        <v>0</v>
-      </c>
-      <c r="F26" s="32">
-        <v>0</v>
-      </c>
-      <c r="G26" s="44"/>
-      <c r="H26" s="32">
-        <v>0</v>
-      </c>
-      <c r="I26" s="51" t="s">
+      <c r="D26" s="30">
+        <v>0</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0</v>
+      </c>
+      <c r="F26" s="30">
+        <v>0</v>
+      </c>
+      <c r="G26" s="42"/>
+      <c r="H26" s="30">
+        <v>0</v>
+      </c>
+      <c r="I26" s="49" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="19">
         <v>4</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="32">
-        <v>0</v>
-      </c>
-      <c r="E27" s="32">
-        <v>0</v>
-      </c>
-      <c r="F27" s="32">
-        <v>0</v>
-      </c>
-      <c r="G27" s="44"/>
-      <c r="H27" s="32">
-        <v>0</v>
-      </c>
-      <c r="I27" s="51" t="s">
+      <c r="D27" s="30">
+        <v>0</v>
+      </c>
+      <c r="E27" s="30">
+        <v>0</v>
+      </c>
+      <c r="F27" s="30">
+        <v>0</v>
+      </c>
+      <c r="G27" s="42"/>
+      <c r="H27" s="30">
+        <v>0</v>
+      </c>
+      <c r="I27" s="49" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="19">
         <v>5</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="32">
-        <v>0</v>
-      </c>
-      <c r="E28" s="32">
-        <v>0</v>
-      </c>
-      <c r="F28" s="32">
-        <v>0</v>
-      </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="32">
-        <v>0</v>
-      </c>
-      <c r="I28" s="51" t="s">
+      <c r="D28" s="30">
+        <v>0</v>
+      </c>
+      <c r="E28" s="30">
+        <v>0</v>
+      </c>
+      <c r="F28" s="30">
+        <v>0</v>
+      </c>
+      <c r="G28" s="42"/>
+      <c r="H28" s="30">
+        <v>0</v>
+      </c>
+      <c r="I28" s="49" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B29" s="19">
         <v>6</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
     </row>
     <row r="47" spans="13:13" x14ac:dyDescent="0.35">
-      <c r="M47" s="6"/>
+      <c r="M47" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3209,7 +3233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D226361B-E2F4-480B-BE87-D86C9E2C81ED}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -3225,58 +3249,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="48" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="19">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>46</v>
       </c>
       <c r="D3">
@@ -3296,39 +3320,39 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="51">
         <v>4</v>
       </c>
-      <c r="E4" s="53">
+      <c r="E4" s="51">
         <v>4</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="51">
         <v>4</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="51">
         <v>4</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D5">
@@ -3348,16 +3372,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="51">
         <v>0</v>
       </c>
       <c r="E6">
@@ -3371,16 +3395,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>4</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="51">
         <v>0.1</v>
       </c>
       <c r="E7">
@@ -3397,25 +3421,25 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <v>5</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="53">
-        <v>0</v>
-      </c>
-      <c r="E8" s="53">
-        <v>0</v>
-      </c>
-      <c r="F8" s="53">
-        <v>0</v>
-      </c>
-      <c r="G8" s="53">
+      <c r="D8" s="51">
+        <v>0</v>
+      </c>
+      <c r="E8" s="51">
+        <v>0</v>
+      </c>
+      <c r="F8" s="51">
+        <v>0</v>
+      </c>
+      <c r="G8" s="51">
         <v>0</v>
       </c>
       <c r="H8">
@@ -3423,16 +3447,16 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="19">
         <v>6</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="53"/>
+      <c r="D9" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add rain-barrel and fix simulate_performances()
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E19C8A6-A007-4282-A2BC-03891DB893EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9696EA-778D-4505-9A0B-9048DA6BFE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" activeTab="1" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" activeTab="3" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="112">
   <si>
     <t>berm.height_mm</t>
   </si>
@@ -586,6 +586,18 @@
   </si>
   <si>
     <t>combi_60percent</t>
+  </si>
+  <si>
+    <t>unknown1</t>
+  </si>
+  <si>
+    <t>unknown2</t>
+  </si>
+  <si>
+    <t>add parameter generated automatically in GUI, otherwise run fails</t>
+  </si>
+  <si>
+    <t>unknown3</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D521626-6D22-40E6-8B80-D0FD83C4D8B0}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -3231,10 +3243,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D226361B-E2F4-480B-BE87-D86C9E2C81ED}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3321,39 +3333,39 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="19">
-        <v>1</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="51">
-        <v>4</v>
-      </c>
-      <c r="E4" s="51">
-        <v>4</v>
-      </c>
-      <c r="F4" s="51">
-        <v>4</v>
-      </c>
-      <c r="G4" s="51">
-        <v>4</v>
-      </c>
-      <c r="H4" s="51">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4">
+        <v>0.75</v>
+      </c>
+      <c r="E4">
+        <v>0.75</v>
+      </c>
+      <c r="F4">
+        <v>0.75</v>
+      </c>
+      <c r="G4">
+        <v>0.75</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="19">
-        <v>2</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>32</v>
+        <v>3</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -3367,31 +3379,34 @@
       <c r="G5">
         <v>0.5</v>
       </c>
-      <c r="H5">
-        <v>0.5</v>
+      <c r="H5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="19">
-        <v>3</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="51">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>600</v>
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3399,25 +3414,25 @@
         <v>29</v>
       </c>
       <c r="B7" s="19">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="51">
         <v>4</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="51">
-        <v>0.1</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
-      <c r="F7">
-        <v>0.1</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
+      <c r="E7" s="51">
+        <v>4</v>
+      </c>
+      <c r="F7" s="51">
+        <v>4</v>
+      </c>
+      <c r="G7" s="51">
+        <v>4</v>
+      </c>
+      <c r="H7" s="51">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3425,25 +3440,25 @@
         <v>29</v>
       </c>
       <c r="B8" s="19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="51">
-        <v>0</v>
-      </c>
-      <c r="E8" s="51">
-        <v>0</v>
-      </c>
-      <c r="F8" s="51">
-        <v>0</v>
-      </c>
-      <c r="G8" s="51">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -3451,12 +3466,101 @@
         <v>29</v>
       </c>
       <c r="B9" s="19">
+        <v>3</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="51">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="F9">
+        <v>400</v>
+      </c>
+      <c r="G9">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="19">
+        <v>4</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="51">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10">
+        <v>0.1</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="19">
+        <v>5</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="51">
+        <v>0</v>
+      </c>
+      <c r="E11" s="51">
+        <v>0</v>
+      </c>
+      <c r="F11" s="51">
+        <v>0</v>
+      </c>
+      <c r="G11" s="51">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="19">
         <v>6</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D12" s="51">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Results for adapted bioretention cell scenarios
developed today together with Kim and Marc (telephone call 2021-07-12)
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9696EA-778D-4505-9A0B-9048DA6BFE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B063D9-4950-4FC1-9830-DCEBBD23C5E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" activeTab="3" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="118">
   <si>
     <t>berm.height_mm</t>
   </si>
@@ -492,12 +492,6 @@
 Loamy sand 0.047 (converted)</t>
   </si>
   <si>
-    <t>mulde_no-drainage</t>
-  </si>
-  <si>
-    <t>mulde_with-drainage</t>
-  </si>
-  <si>
     <t>scenario: with/without</t>
   </si>
   <si>
@@ -561,12 +555,6 @@
     <t>https://cloud.kompetenz-wasser.de/index.php/f/180255</t>
   </si>
   <si>
-    <t>mulde_rigole_no-drainage</t>
-  </si>
-  <si>
-    <t>mulde_rigole_with-drainage</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
@@ -598,6 +586,36 @@
   </si>
   <si>
     <t>unknown3</t>
+  </si>
+  <si>
+    <t>36mm.per.hour_mulde_no-drainage</t>
+  </si>
+  <si>
+    <t>36mm.per.hour_mulde_rigole_no-drainage</t>
+  </si>
+  <si>
+    <t>36mm.per.hour_mulde_rigole_with-drainage</t>
+  </si>
+  <si>
+    <t>360mm.per.hour_mulde_no-drainage</t>
+  </si>
+  <si>
+    <t>360mm.per.hour_mulde_rigole_no-drainage</t>
+  </si>
+  <si>
+    <t>360mm.per.hour_mulde_rigole_with-drainage</t>
+  </si>
+  <si>
+    <t>3600mm.per.hour_mulde_no-drainage</t>
+  </si>
+  <si>
+    <t>3.6mm.per.hour_mulde_no-drainage</t>
+  </si>
+  <si>
+    <t>3.6mm.per.hour_mulde_rigole_no-drainage</t>
+  </si>
+  <si>
+    <t>3.6mm.per.hour_mulde_rigole_with-drainage</t>
   </si>
 </sst>
 </file>
@@ -1248,13 +1266,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F4C19-D880-47FC-8424-E4A612FEC51C}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14:E17"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1263,45 +1281,65 @@
     <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.453125" customWidth="1"/>
-    <col min="7" max="7" width="50.1796875" customWidth="1"/>
-    <col min="8" max="8" width="78" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.1796875" customWidth="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.453125" customWidth="1"/>
+    <col min="9" max="13" width="50.1796875" customWidth="1"/>
+    <col min="14" max="14" width="78" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="O1" s="48" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="34" t="s">
@@ -1310,15 +1348,21 @@
       <c r="D2" s="32"/>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -1334,20 +1378,38 @@
       <c r="E3">
         <v>300</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="35">
         <v>300</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3">
         <v>300</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3">
+        <v>300</v>
+      </c>
+      <c r="I3" s="35">
+        <v>300</v>
+      </c>
+      <c r="J3">
+        <v>300</v>
+      </c>
+      <c r="K3">
+        <v>300</v>
+      </c>
+      <c r="L3" s="35">
+        <v>300</v>
+      </c>
+      <c r="M3">
+        <v>300</v>
+      </c>
+      <c r="N3" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="I3" t="s">
+      <c r="O3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -1369,14 +1431,32 @@
       <c r="G4" s="35">
         <v>0.05</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="I4" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="J4" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="K4" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="L4" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="M4" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="N4" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="I4" t="s">
+      <c r="O4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
@@ -1398,14 +1478,32 @@
       <c r="G5">
         <v>0.3</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>0.3</v>
+      </c>
+      <c r="I5">
+        <v>0.3</v>
+      </c>
+      <c r="J5">
+        <v>0.3</v>
+      </c>
+      <c r="K5">
+        <v>0.3</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+      <c r="M5">
+        <v>0.3</v>
+      </c>
+      <c r="N5" t="s">
         <v>52</v>
       </c>
-      <c r="I5" t="s">
+      <c r="O5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
@@ -1427,14 +1525,32 @@
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
         <v>59</v>
       </c>
-      <c r="I6" t="s">
+      <c r="O6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
@@ -1456,14 +1572,32 @@
       <c r="G7">
         <v>500</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <v>500</v>
+      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+      <c r="J7">
+        <v>500</v>
+      </c>
+      <c r="K7">
+        <v>500</v>
+      </c>
+      <c r="L7">
+        <v>500</v>
+      </c>
+      <c r="M7">
+        <v>500</v>
+      </c>
+      <c r="N7" t="s">
         <v>63</v>
       </c>
-      <c r="I7" t="s">
+      <c r="O7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
@@ -1485,14 +1619,32 @@
       <c r="G8">
         <v>0.437</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8">
+        <v>0.437</v>
+      </c>
+      <c r="I8">
+        <v>0.437</v>
+      </c>
+      <c r="J8">
+        <v>0.437</v>
+      </c>
+      <c r="K8">
+        <v>0.437</v>
+      </c>
+      <c r="L8">
+        <v>0.437</v>
+      </c>
+      <c r="M8">
+        <v>0.437</v>
+      </c>
+      <c r="N8" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="I8" t="s">
+      <c r="O8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1514,14 +1666,32 @@
       <c r="G9" s="35">
         <v>0.105</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="35">
+        <v>0.105</v>
+      </c>
+      <c r="I9" s="35">
+        <v>0.105</v>
+      </c>
+      <c r="J9" s="35">
+        <v>0.105</v>
+      </c>
+      <c r="K9" s="35">
+        <v>0.105</v>
+      </c>
+      <c r="L9" s="35">
+        <v>0.105</v>
+      </c>
+      <c r="M9" s="35">
+        <v>0.105</v>
+      </c>
+      <c r="N9" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="I9" t="s">
+      <c r="O9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1543,14 +1713,32 @@
       <c r="G10">
         <v>4.7E-2</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="K10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="M10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="N10" t="s">
         <v>71</v>
       </c>
-      <c r="I10" t="s">
+      <c r="O10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -1561,22 +1749,40 @@
         <v>6</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>3.6</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>3600</v>
       </c>
       <c r="F11">
-        <v>30</v>
+        <v>3600</v>
       </c>
       <c r="G11">
-        <v>30</v>
-      </c>
-      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11">
+        <v>3600</v>
+      </c>
+      <c r="I11">
+        <v>3600</v>
+      </c>
+      <c r="J11">
+        <v>360</v>
+      </c>
+      <c r="K11">
+        <v>3600</v>
+      </c>
+      <c r="L11">
+        <v>3600</v>
+      </c>
+      <c r="M11">
+        <v>3600</v>
+      </c>
+      <c r="O11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
@@ -1598,14 +1804,32 @@
       <c r="G12">
         <v>0.5</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12">
+        <v>0.5</v>
+      </c>
+      <c r="K12">
+        <v>0.5</v>
+      </c>
+      <c r="L12">
+        <v>0.5</v>
+      </c>
+      <c r="M12">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="I12" t="s">
+      <c r="O12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -1627,14 +1851,32 @@
       <c r="G13">
         <v>4.7E-2</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="K13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="M13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="N13" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="I13" t="s">
+      <c r="O13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
         <v>27</v>
       </c>
@@ -1644,20 +1886,32 @@
       <c r="C14" s="20" t="s">
         <v>2</v>
       </c>
+      <c r="E14">
+        <v>250</v>
+      </c>
       <c r="F14">
         <v>250</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>250</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14">
+        <v>250</v>
+      </c>
+      <c r="K14">
+        <v>250</v>
+      </c>
+      <c r="L14">
+        <v>250</v>
+      </c>
+      <c r="N14" t="s">
         <v>54</v>
       </c>
-      <c r="I14" t="s">
+      <c r="O14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>27</v>
       </c>
@@ -1667,20 +1921,32 @@
       <c r="C15" s="20" t="s">
         <v>21</v>
       </c>
+      <c r="E15">
+        <v>0.6</v>
+      </c>
       <c r="F15">
         <v>0.6</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.6</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15">
+        <v>0.6</v>
+      </c>
+      <c r="K15">
+        <v>0.6</v>
+      </c>
+      <c r="L15">
+        <v>0.6</v>
+      </c>
+      <c r="N15" t="s">
         <v>53</v>
       </c>
-      <c r="I15" t="s">
+      <c r="O15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
@@ -1690,20 +1956,32 @@
       <c r="C16" s="20" t="s">
         <v>30</v>
       </c>
+      <c r="E16">
+        <v>3.6</v>
+      </c>
       <c r="F16">
-        <v>7.43</v>
-      </c>
-      <c r="G16">
-        <v>7.43</v>
-      </c>
-      <c r="H16" t="s">
+        <v>3.6</v>
+      </c>
+      <c r="H16">
+        <v>36</v>
+      </c>
+      <c r="I16">
+        <v>36</v>
+      </c>
+      <c r="K16">
+        <v>360</v>
+      </c>
+      <c r="L16">
+        <v>360</v>
+      </c>
+      <c r="N16" t="s">
         <v>55</v>
       </c>
-      <c r="I16" t="s">
+      <c r="O16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
@@ -1713,17 +1991,29 @@
       <c r="C17" s="21" t="s">
         <v>24</v>
       </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
@@ -1733,17 +2023,20 @@
       <c r="C18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>2</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>2</v>
       </c>
-      <c r="I18" t="s">
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="O18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
         <v>29</v>
       </c>
@@ -1753,14 +2046,17 @@
       <c r="C19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>0.5</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>29</v>
       </c>
@@ -1770,14 +2066,17 @@
       <c r="C20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>100</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
         <v>29</v>
       </c>
@@ -1787,14 +2086,17 @@
       <c r="C21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
         <v>29</v>
       </c>
@@ -1804,14 +2106,17 @@
       <c r="C22" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>29</v>
       </c>
@@ -1851,34 +2156,34 @@
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>84</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>61</v>
@@ -2004,7 +2309,7 @@
         <v>50</v>
       </c>
       <c r="M4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2045,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -2086,7 +2391,7 @@
         <v>80</v>
       </c>
       <c r="M6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.35">
@@ -2127,7 +2432,7 @@
         <v>18</v>
       </c>
       <c r="M7" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -2168,7 +2473,7 @@
         <v>0.35</v>
       </c>
       <c r="M8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -2209,7 +2514,7 @@
         <v>0.05</v>
       </c>
       <c r="M9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
@@ -2250,7 +2555,7 @@
         <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -2291,7 +2596,7 @@
         <v>30</v>
       </c>
       <c r="M11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2332,7 +2637,7 @@
         <v>10</v>
       </c>
       <c r="M12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -2373,7 +2678,7 @@
         <v>40</v>
       </c>
       <c r="M13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -2414,7 +2719,7 @@
         <v>49</v>
       </c>
       <c r="M14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -2455,7 +2760,7 @@
         <v>28</v>
       </c>
       <c r="M15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2469,10 +2774,10 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2492,7 +2797,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>14</v>
@@ -3104,7 +3409,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3131,7 +3436,7 @@
         <v>0.4</v>
       </c>
       <c r="I25" s="49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -3158,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -3185,7 +3490,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -3212,7 +3517,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -3245,7 +3550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D226361B-E2F4-480B-BE87-D86C9E2C81ED}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -3265,22 +3570,22 @@
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>61</v>
@@ -3291,7 +3596,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="34" t="s">
@@ -3302,7 +3607,7 @@
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
       <c r="H2" s="33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3339,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D4">
         <v>0.75</v>
@@ -3354,7 +3659,7 @@
         <v>0.75</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -3365,7 +3670,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -3380,7 +3685,7 @@
         <v>0.5</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3391,7 +3696,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3406,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3559,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed green-roof parameterisation error
mixed up intensive_no-drainmat and intensive_with-drainmat

to do: re-run performance calculation
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B063D9-4950-4FC1-9830-DCEBBD23C5E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEAFDB5-0910-467D-B956-338A8E1A48E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="1" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -1268,29 +1268,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F4C19-D880-47FC-8424-E4A612FEC51C}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" customWidth="1"/>
-    <col min="6" max="6" width="50.1796875" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
     <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.453125" customWidth="1"/>
-    <col min="9" max="13" width="50.1796875" customWidth="1"/>
+    <col min="8" max="8" width="51.42578125" customWidth="1"/>
+    <col min="9" max="13" width="50.140625" customWidth="1"/>
     <col min="14" max="14" width="78" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>97</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>27</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>27</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>29</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>29</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>29</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>29</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>29</v>
       </c>
@@ -2137,21 +2137,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D521626-6D22-40E6-8B80-D0FD83C4D8B0}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="48.81640625" customWidth="1"/>
-    <col min="7" max="11" width="45.453125" customWidth="1"/>
-    <col min="12" max="13" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="48.85546875" customWidth="1"/>
+    <col min="7" max="11" width="45.42578125" customWidth="1"/>
+    <col min="12" max="13" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>10</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
@@ -2657,10 +2657,10 @@
         <v>40</v>
       </c>
       <c r="F13" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="11">
         <v>80</v>
-      </c>
-      <c r="G13" s="11">
-        <v>0.1</v>
       </c>
       <c r="H13" s="11">
         <v>0.1</v>
@@ -2681,7 +2681,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -2780,19 +2780,19 @@
       <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" style="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.81640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.81640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="I2" s="23"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -2875,7 +2875,7 @@
       </c>
       <c r="I3" s="23"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>20</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>20</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>20</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>20</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>10</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>10</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>10</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>10</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>10</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>27</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>27</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>27</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>27</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>29</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>29</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>29</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>29</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>29</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>29</v>
       </c>
@@ -3537,7 +3537,7 @@
       <c r="H29" s="47"/>
       <c r="I29" s="47"/>
     </row>
-    <row r="47" spans="13:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M47" s="5"/>
     </row>
   </sheetData>
@@ -3554,18 +3554,18 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.1796875" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>97</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>27</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>29</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>29</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>29</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
bioretention-cells: fix parameterisation :bug:
"conductivity_mm.per.hour" was not in line with scenario name before due to wrong parametert definition in EXCEL file
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEAFDB5-0910-467D-B956-338A8E1A48E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78833A13-AB7B-4F6C-990F-1E793A05B915}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" activeTab="1" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="bioretention_cell" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="106">
   <si>
     <t>berm.height_mm</t>
   </si>
@@ -517,42 +517,6 @@
   </si>
   <si>
     <t>with-berm_intensive_with-drainmat</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180244</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180245</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180246</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180247</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180248</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180249</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180250</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180251</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180252</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180253</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180254</t>
-  </si>
-  <si>
-    <t>https://cloud.kompetenz-wasser.de/index.php/f/180255</t>
   </si>
   <si>
     <t>area</t>
@@ -1268,67 +1232,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97F4C19-D880-47FC-8424-E4A612FEC51C}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" customWidth="1"/>
+    <col min="6" max="6" width="50.1796875" customWidth="1"/>
     <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.42578125" customWidth="1"/>
-    <col min="9" max="13" width="50.140625" customWidth="1"/>
+    <col min="8" max="8" width="51.453125" customWidth="1"/>
+    <col min="9" max="13" width="50.1796875" customWidth="1"/>
     <col min="14" max="14" width="78" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="N1" s="16" t="s">
         <v>61</v>
@@ -1337,9 +1301,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="34" t="s">
@@ -1362,7 +1326,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -1409,7 +1373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
@@ -1503,7 +1467,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
@@ -1550,7 +1514,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
@@ -1597,7 +1561,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
@@ -1644,7 +1608,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1691,7 +1655,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -1738,7 +1702,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>10</v>
       </c>
@@ -1752,28 +1716,28 @@
         <v>3.6</v>
       </c>
       <c r="E11">
-        <v>3600</v>
+        <v>3.6</v>
       </c>
       <c r="F11">
-        <v>3600</v>
+        <v>3.6</v>
       </c>
       <c r="G11">
         <v>36</v>
       </c>
       <c r="H11">
-        <v>3600</v>
+        <v>36</v>
       </c>
       <c r="I11">
-        <v>3600</v>
+        <v>36</v>
       </c>
       <c r="J11">
         <v>360</v>
       </c>
       <c r="K11">
-        <v>3600</v>
+        <v>360</v>
       </c>
       <c r="L11">
-        <v>3600</v>
+        <v>360</v>
       </c>
       <c r="M11">
         <v>3600</v>
@@ -1782,7 +1746,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
@@ -1829,7 +1793,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -1876,7 +1840,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
         <v>27</v>
       </c>
@@ -1911,7 +1875,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>27</v>
       </c>
@@ -1946,7 +1910,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1945,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>27</v>
       </c>
@@ -2013,7 +1977,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
@@ -2036,7 +2000,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
         <v>29</v>
       </c>
@@ -2056,7 +2020,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>29</v>
       </c>
@@ -2076,7 +2040,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
         <v>29</v>
       </c>
@@ -2096,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
         <v>29</v>
       </c>
@@ -2116,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>29</v>
       </c>
@@ -2137,26 +2101,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D521626-6D22-40E6-8B80-D0FD83C4D8B0}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="J1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="48.85546875" customWidth="1"/>
-    <col min="7" max="11" width="45.42578125" customWidth="1"/>
-    <col min="12" max="13" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="48.81640625" customWidth="1"/>
+    <col min="7" max="11" width="45.453125" customWidth="1"/>
+    <col min="12" max="13" width="48.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>14</v>
@@ -2192,7 +2156,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -2230,7 +2194,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -2267,11 +2231,11 @@
       <c r="L3" s="7">
         <v>0.15</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -2308,11 +2272,11 @@
       <c r="L4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="M4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -2349,11 +2313,11 @@
       <c r="L5" s="7">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="52" t="s">
         <v>10</v>
       </c>
@@ -2390,11 +2354,11 @@
       <c r="L6" s="54">
         <v>80</v>
       </c>
-      <c r="M6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -2431,11 +2395,11 @@
       <c r="L7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -2472,11 +2436,11 @@
       <c r="L8" s="7">
         <v>0.35</v>
       </c>
-      <c r="M8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -2513,11 +2477,11 @@
       <c r="L9" s="7">
         <v>0.05</v>
       </c>
-      <c r="M9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -2554,11 +2518,11 @@
       <c r="L10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -2595,11 +2559,11 @@
       <c r="L11" s="7">
         <v>30</v>
       </c>
-      <c r="M11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
@@ -2636,11 +2600,11 @@
       <c r="L12" s="15">
         <v>10</v>
       </c>
-      <c r="M12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
@@ -2677,11 +2641,11 @@
       <c r="L13" s="11">
         <v>40</v>
       </c>
-      <c r="M13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -2718,11 +2682,11 @@
       <c r="L14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -2759,13 +2723,28 @@
       <c r="L15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M15" t="s">
-        <v>96</v>
+      <c r="M15" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{23B6A44B-93EA-4097-84A5-7DB5D8C804FE}"/>
+    <hyperlink ref="M5" r:id="rId2" xr:uid="{8D01ED8E-58D7-42E8-8BC4-12C54C4B85BF}"/>
+    <hyperlink ref="M7" r:id="rId3" xr:uid="{08A91F93-6E9D-4B57-B0E4-E8EDFDA0F758}"/>
+    <hyperlink ref="M9" r:id="rId4" xr:uid="{0798FB2A-1F7F-4CAA-8FC3-E2C5A995CD5A}"/>
+    <hyperlink ref="M11" r:id="rId5" xr:uid="{12FE61D1-6C38-4635-B259-3409BD51515D}"/>
+    <hyperlink ref="M13" r:id="rId6" xr:uid="{17385853-D798-45B2-926F-F6F3789F3E25}"/>
+    <hyperlink ref="M15" r:id="rId7" xr:uid="{E1383B61-D399-4CFA-8DF3-159E0B33FFCD}"/>
+    <hyperlink ref="M4" r:id="rId8" xr:uid="{ECC9D49A-B3BE-4210-ACC9-F3F41C656EAC}"/>
+    <hyperlink ref="M6" r:id="rId9" xr:uid="{AEB985CB-695D-4BE1-A8E9-C1443656ED62}"/>
+    <hyperlink ref="M8" r:id="rId10" xr:uid="{E338BCAE-E1E5-47A1-8F1E-E87C65286654}"/>
+    <hyperlink ref="M10" r:id="rId11" xr:uid="{FA93CC56-DF82-4828-A329-347C6F178B33}"/>
+    <hyperlink ref="M12" r:id="rId12" xr:uid="{BA2F5590-0427-417A-B5E4-8F6CE02038AA}"/>
+    <hyperlink ref="M14" r:id="rId13" xr:uid="{FC8502E7-F1B5-429D-80A0-571F8F30719A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -2774,30 +2753,30 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.81640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.81640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>14</v>
@@ -2821,7 +2800,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
@@ -2848,7 +2827,7 @@
       </c>
       <c r="I2" s="23"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -2875,7 +2854,7 @@
       </c>
       <c r="I3" s="23"/>
     </row>
-    <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -2904,7 +2883,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
@@ -2933,7 +2912,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>20</v>
       </c>
@@ -2962,7 +2941,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>20</v>
       </c>
@@ -2991,7 +2970,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>20</v>
       </c>
@@ -3020,7 +2999,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>20</v>
       </c>
@@ -3049,7 +3028,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>20</v>
       </c>
@@ -3078,7 +3057,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>20</v>
       </c>
@@ -3107,7 +3086,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
@@ -3136,7 +3115,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
@@ -3155,7 +3134,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
@@ -3174,7 +3153,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>10</v>
       </c>
@@ -3193,7 +3172,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="19" t="s">
         <v>10</v>
       </c>
@@ -3212,7 +3191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="19" t="s">
         <v>10</v>
       </c>
@@ -3231,7 +3210,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>10</v>
       </c>
@@ -3250,7 +3229,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
         <v>10</v>
       </c>
@@ -3269,7 +3248,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>27</v>
       </c>
@@ -3298,7 +3277,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
         <v>27</v>
       </c>
@@ -3327,7 +3306,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
         <v>27</v>
       </c>
@@ -3356,7 +3335,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>27</v>
       </c>
@@ -3385,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
         <v>29</v>
       </c>
@@ -3412,7 +3391,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>29</v>
       </c>
@@ -3439,7 +3418,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>29</v>
       </c>
@@ -3466,7 +3445,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="19" t="s">
         <v>29</v>
       </c>
@@ -3493,7 +3472,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
         <v>29</v>
       </c>
@@ -3520,7 +3499,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="19" t="s">
         <v>29</v>
       </c>
@@ -3537,7 +3516,7 @@
       <c r="H29" s="47"/>
       <c r="I29" s="47"/>
     </row>
-    <row r="47" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="13:13" x14ac:dyDescent="0.35">
       <c r="M47" s="5"/>
     </row>
   </sheetData>
@@ -3554,38 +3533,38 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.453125" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>61</v>
@@ -3594,9 +3573,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="34" t="s">
@@ -3607,10 +3586,10 @@
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
       <c r="H2" s="33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
@@ -3636,7 +3615,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -3644,7 +3623,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D4">
         <v>0.75</v>
@@ -3659,10 +3638,10 @@
         <v>0.75</v>
       </c>
       <c r="H4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>27</v>
       </c>
@@ -3670,7 +3649,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -3685,10 +3664,10 @@
         <v>0.5</v>
       </c>
       <c r="H5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
@@ -3696,7 +3675,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3711,10 +3690,10 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
@@ -3740,7 +3719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
@@ -3766,7 +3745,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>29</v>
       </c>
@@ -3789,7 +3768,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>29</v>
       </c>
@@ -3815,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>29</v>
       </c>
@@ -3841,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>29</v>
       </c>
@@ -3864,7 +3843,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename "German" scenario names to "English"
for bioretention cells
</commit_message>
<xml_diff>
--- a/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
+++ b/inst/extdata/scenarios/swmm_lid-parameterisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrustl\Documents\RProjects\keys.lid\inst\extdata\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78833A13-AB7B-4F6C-990F-1E793A05B915}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF0DC0A-7652-483D-95A1-23A371362F13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11330" xr2:uid="{2C0CC149-430D-45D4-BA68-435A859DB6BA}"/>
   </bookViews>
@@ -552,34 +552,34 @@
     <t>unknown3</t>
   </si>
   <si>
-    <t>36mm.per.hour_mulde_no-drainage</t>
-  </si>
-  <si>
-    <t>36mm.per.hour_mulde_rigole_no-drainage</t>
-  </si>
-  <si>
-    <t>36mm.per.hour_mulde_rigole_with-drainage</t>
-  </si>
-  <si>
-    <t>360mm.per.hour_mulde_no-drainage</t>
-  </si>
-  <si>
-    <t>360mm.per.hour_mulde_rigole_no-drainage</t>
-  </si>
-  <si>
-    <t>360mm.per.hour_mulde_rigole_with-drainage</t>
-  </si>
-  <si>
-    <t>3600mm.per.hour_mulde_no-drainage</t>
-  </si>
-  <si>
-    <t>3.6mm.per.hour_mulde_no-drainage</t>
-  </si>
-  <si>
-    <t>3.6mm.per.hour_mulde_rigole_no-drainage</t>
-  </si>
-  <si>
-    <t>3.6mm.per.hour_mulde_rigole_with-drainage</t>
+    <t>360mm.per.hour_through-trench_no-drainage</t>
+  </si>
+  <si>
+    <t>360mm.per.hour_through-trench_with-drainage</t>
+  </si>
+  <si>
+    <t>3.6mm.per.hour_through-trench_no-drainage</t>
+  </si>
+  <si>
+    <t>3.6mm.per.hour_through-trench_with-drainage</t>
+  </si>
+  <si>
+    <t>36mm.per.hour_through-trench_no-drainage</t>
+  </si>
+  <si>
+    <t>36mm.per.hour_through-trench_with-drainage</t>
+  </si>
+  <si>
+    <t>3.6mm.per.hour_through_no-drainage</t>
+  </si>
+  <si>
+    <t>36mm.per.hour_through_no-drainage</t>
+  </si>
+  <si>
+    <t>360mm.per.hour_through_no-drainage</t>
+  </si>
+  <si>
+    <t>3600mm.per.hour_through_no-drainage</t>
   </si>
 </sst>
 </file>
@@ -1233,10 +1233,10 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1265,34 +1265,34 @@
         <v>14</v>
       </c>
       <c r="D1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="H1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="K1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>102</v>
       </c>
       <c r="N1" s="16" t="s">
         <v>61</v>

</xml_diff>